<commit_message>
hal of pair mode done; font size in buttons correct
</commit_message>
<xml_diff>
--- a/Discover China 1 all vocabulary.xlsx
+++ b/Discover China 1 all vocabulary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Discover China\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F799DDC-720A-4936-B91F-1366DAC232B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3F9CB8-75B8-48BF-999A-26354CF01B52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7EBEC6ED-38C4-453E-AFF8-D89EE891FB41}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="11" xr2:uid="{7EBEC6ED-38C4-453E-AFF8-D89EE891FB41}"/>
   </bookViews>
   <sheets>
     <sheet name="unit 1" sheetId="1" r:id="rId1"/>
@@ -1139,9 +1139,6 @@
     <t>gōngyù</t>
   </si>
   <si>
-    <t>block of flats, apartment building</t>
-  </si>
-  <si>
     <r>
       <t>房间</t>
     </r>
@@ -5461,6 +5458,9 @@
   </si>
   <si>
     <t>大家</t>
+  </si>
+  <si>
+    <t>block of flats</t>
   </si>
 </sst>
 </file>
@@ -5862,7 +5862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5861C5B0-94EA-4FFD-86ED-C28A1C4EF31F}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -6095,7 +6095,7 @@
     </row>
     <row r="21" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>203</v>
@@ -6122,280 +6122,280 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>132</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>766</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>767</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>769</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>770</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>772</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>773</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>774</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>775</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>776</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>141</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>780</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>782</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>783</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>784</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>785</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>787</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>788</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>790</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>791</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>793</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>794</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>796</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>797</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>798</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>799</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>801</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>802</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>804</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>805</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>807</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>808</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>810</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>811</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>813</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>814</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>816</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>817</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>819</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>820</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>822</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>823</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>825</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>826</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>828</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>829</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>830</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>831</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>832</v>
       </c>
     </row>
   </sheetData>
@@ -6418,310 +6418,310 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>840</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>897</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>842</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>898</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>843</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>844</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>899</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>845</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>846</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>900</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>848</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>901</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>850</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>703</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
+        <v>851</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>852</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>902</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>853</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>854</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>903</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>856</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>904</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
+        <v>857</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>858</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>905</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>859</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>860</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>906</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>862</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>907</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>864</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>908</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
+        <v>865</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>866</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>909</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>868</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>910</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>869</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -6738,7 +6738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D79124-9754-4A69-B150-B37F221C3809}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -6746,142 +6746,142 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>922</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>923</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>925</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>926</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>928</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>929</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>931</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>932</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>934</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>935</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>937</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>938</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>940</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>941</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>943</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>944</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>946</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>947</v>
-      </c>
       <c r="C9" s="2" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>949</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>950</v>
-      </c>
       <c r="C10" s="2" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>952</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>953</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>955</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>956</v>
-      </c>
       <c r="C12" s="2" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>957</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>958</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>218</v>
@@ -6889,211 +6889,211 @@
     </row>
     <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>960</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>961</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>963</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>964</v>
-      </c>
       <c r="C15" s="2" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>966</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>967</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>969</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>970</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>972</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>973</v>
-      </c>
       <c r="C18" s="2" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>975</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>976</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>978</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>979</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>981</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>982</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>984</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>985</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>987</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>988</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>990</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>991</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>993</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>994</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>996</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>997</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>999</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>1000</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>1002</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>1003</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>1005</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>1006</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>1008</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>1009</v>
-      </c>
       <c r="C30" s="2" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>1011</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>1012</v>
-      </c>
       <c r="C31" s="2" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>1014</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>1015</v>
-      </c>
       <c r="C32" s="2" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
   </sheetData>
@@ -7105,7 +7105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{838E1262-2533-4393-9BBD-7FEC2E101BB9}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -7400,7 +7400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA9FF72-088C-4BD6-8A7D-60B0AAF98CB3}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -7726,7 +7726,7 @@
         <v>217</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -7938,7 +7938,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8064,84 +8064,84 @@
         <v>305</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>306</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -8153,7 +8153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444AC4B1-DDCA-41A0-B0A0-75137B0997FC}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -8161,389 +8161,389 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>341</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>347</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>349</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>352</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>358</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>379</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>382</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>403</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>406</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>411</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>417</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -8555,7 +8555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118E476F-4901-4D4D-8D96-0042DB185D0C}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -8563,10 +8563,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>92</v>
@@ -8574,467 +8574,467 @@
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>438</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>444</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>447</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>453</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>456</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>459</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>468</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>471</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>474</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>476</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>477</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>483</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>486</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>488</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>490</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>491</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>493</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>494</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>200</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>499</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>502</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>505</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>507</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>513</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>516</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>519</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>522</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>525</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>528</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>531</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>534</v>
-      </c>
       <c r="C36" s="2" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>535</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>536</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>539</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>542</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>545</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>548</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>550</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>551</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>554</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -9054,432 +9054,432 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>556</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>557</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>560</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>563</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>565</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>566</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>569</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>572</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>575</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>578</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>587</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>200</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>592</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>598</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>601</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>604</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>607</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>610</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>613</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>616</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>618</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>621</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>624</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>627</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>630</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>636</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>639</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>642</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>645</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>648</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>651</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>653</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>656</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>659</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>662</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>665</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>668</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>669</v>
       </c>
     </row>
   </sheetData>
@@ -9499,10 +9499,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>671</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>672</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>48</v>
@@ -9510,343 +9510,343 @@
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>674</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>677</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>680</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>683</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>686</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>689</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>691</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>692</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>695</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>698</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>700</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>701</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>703</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>706</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>708</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>709</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>711</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>712</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>715</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>716</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>717</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>720</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>722</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>723</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>724</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>725</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>726</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>729</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>732</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>734</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>735</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>737</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>738</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>740</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>741</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>743</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>744</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>746</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>747</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>749</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>750</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>753</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>756</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>759</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>761</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>762</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>763</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished choose keys mode
</commit_message>
<xml_diff>
--- a/Discover China 1 all vocabulary.xlsx
+++ b/Discover China 1 all vocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Discover China\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3F9CB8-75B8-48BF-999A-26354CF01B52}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF53653E-2360-40B7-89F4-D52ECD69C9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="11" xr2:uid="{7EBEC6ED-38C4-453E-AFF8-D89EE891FB41}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="12" xr2:uid="{7EBEC6ED-38C4-453E-AFF8-D89EE891FB41}"/>
   </bookViews>
   <sheets>
     <sheet name="unit 1" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="unit 10" sheetId="10" r:id="rId10"/>
     <sheet name="unit 11" sheetId="11" r:id="rId11"/>
     <sheet name="unit 12" sheetId="12" r:id="rId12"/>
+    <sheet name="keys" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="1376">
   <si>
     <t>hello</t>
   </si>
@@ -5461,13 +5462,1087 @@
   </si>
   <si>
     <t>block of flats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">一 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yī </t>
+  </si>
+  <si>
+    <t xml:space="preserve">丨 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gǔn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> вертикальная</t>
+  </si>
+  <si>
+    <t xml:space="preserve">丶 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zhǔ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> точка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">丿 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> piě </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> откидная влево</t>
+  </si>
+  <si>
+    <t xml:space="preserve">乙，乚 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yǐ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> второй</t>
+  </si>
+  <si>
+    <t xml:space="preserve">亅 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jué </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> вертикальная с крюком</t>
+  </si>
+  <si>
+    <t xml:space="preserve">二 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> èr </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> два</t>
+  </si>
+  <si>
+    <t xml:space="preserve">亠 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tóu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> горизонтальная с точкой</t>
+  </si>
+  <si>
+    <t>https://quizlet.com/ru/559702440/chinese-keys-flash-cards/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">人，亻 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rén </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> человек</t>
+  </si>
+  <si>
+    <t xml:space="preserve">儿 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ér </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> идущий чедовек</t>
+  </si>
+  <si>
+    <t xml:space="preserve">入 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rù </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> входить</t>
+  </si>
+  <si>
+    <t xml:space="preserve">八 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bā </t>
+  </si>
+  <si>
+    <t xml:space="preserve">冂 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jiōng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> граница</t>
+  </si>
+  <si>
+    <t xml:space="preserve">冖 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mì </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> крышка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">冫 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bīng </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> лед</t>
+  </si>
+  <si>
+    <t xml:space="preserve">几 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jī </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> стол</t>
+  </si>
+  <si>
+    <t xml:space="preserve">凵 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kǎn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> яма</t>
+  </si>
+  <si>
+    <t xml:space="preserve">刀，刂 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dāo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> нож</t>
+  </si>
+  <si>
+    <t xml:space="preserve">力 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> lì </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> сила</t>
+  </si>
+  <si>
+    <t xml:space="preserve">勹 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bāo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> обертывать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">匕 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bǐ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> черпак, кинжал</t>
+  </si>
+  <si>
+    <t xml:space="preserve">匚 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fāng </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ящик, короб</t>
+  </si>
+  <si>
+    <t xml:space="preserve">匸 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xì</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> прятать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">十 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shí </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> десять</t>
+  </si>
+  <si>
+    <t xml:space="preserve">卜 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bǔ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> гадать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">卩， 㔾 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jié </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> печать, власть</t>
+  </si>
+  <si>
+    <t xml:space="preserve">厂 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hǎn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> обрыв, круча</t>
+  </si>
+  <si>
+    <t xml:space="preserve">厶 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sī </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> частный, личный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">又 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yòu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> правая рука, опять</t>
+  </si>
+  <si>
+    <t xml:space="preserve">口 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> kǒu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> рот</t>
+  </si>
+  <si>
+    <t xml:space="preserve">囗 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wéi </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> окружать, ограда</t>
+  </si>
+  <si>
+    <t xml:space="preserve">土 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tǔ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> земля</t>
+  </si>
+  <si>
+    <t xml:space="preserve">士 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shì </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> воин</t>
+  </si>
+  <si>
+    <t xml:space="preserve">夂 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zhǐ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">夊 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> suī </t>
+  </si>
+  <si>
+    <t xml:space="preserve">夕 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xī </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> вечер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">大 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dà </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> большой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">女 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nǚ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> женщина</t>
+  </si>
+  <si>
+    <t xml:space="preserve">子 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zǐ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ребенок, сын</t>
+  </si>
+  <si>
+    <t xml:space="preserve">宀 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mián </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> крыша с точкой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">寸 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cùn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> вершок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">小 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xiǎo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> маленький</t>
+  </si>
+  <si>
+    <t xml:space="preserve">尢，尣 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wāng </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> хромой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">尸 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shī</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> труп</t>
+  </si>
+  <si>
+    <t xml:space="preserve">屮 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chè </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> росток</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shān </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> гора</t>
+  </si>
+  <si>
+    <t xml:space="preserve">巛，川 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chuān </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> поток, река</t>
+  </si>
+  <si>
+    <t xml:space="preserve">工 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gōng </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> работа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">己，已，巳 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jǐ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> сам</t>
+  </si>
+  <si>
+    <t xml:space="preserve">巾 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jīn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> полотенце</t>
+  </si>
+  <si>
+    <t xml:space="preserve">干 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gān </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> щит, вмешиваться</t>
+  </si>
+  <si>
+    <t xml:space="preserve">幺 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yāo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> незрелый, младший</t>
+  </si>
+  <si>
+    <t xml:space="preserve">广 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yǎn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> навес, укрытие</t>
+  </si>
+  <si>
+    <t xml:space="preserve">廴 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yǐn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> двигаться вперед, тащить</t>
+  </si>
+  <si>
+    <t xml:space="preserve">廾 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gǒng </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> соединить руки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">弋 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yì </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> стрелять из лука</t>
+  </si>
+  <si>
+    <t xml:space="preserve">弓 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> лук (оружие)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">彐，彑 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jì </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> голова свиньи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">彡 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> перья, длинна шерсть</t>
+  </si>
+  <si>
+    <t xml:space="preserve">彳 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chì </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> шаг</t>
+  </si>
+  <si>
+    <t xml:space="preserve">心，忄，㣺 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xīn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> сердце</t>
+  </si>
+  <si>
+    <t xml:space="preserve">戈 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gē </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> копье, клевец</t>
+  </si>
+  <si>
+    <t xml:space="preserve">户，戸，戶 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hù </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> двор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">手，扌 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shǒu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> рука</t>
+  </si>
+  <si>
+    <t xml:space="preserve">支 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zhī </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ветка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">攴，攵 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pū </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> бить, ударять</t>
+  </si>
+  <si>
+    <t xml:space="preserve">文 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wén </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> текст, письмена</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斗 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dǒu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ковш, хлебная мерка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">斤 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> топор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">方 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> квадрат, сторона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">无 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wú </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> не, без</t>
+  </si>
+  <si>
+    <t xml:space="preserve">日 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rì </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> солнце</t>
+  </si>
+  <si>
+    <t xml:space="preserve">曰 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yuē </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> говорить</t>
+  </si>
+  <si>
+    <t xml:space="preserve">月 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yuè </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> луна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">木 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mù </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> дерево</t>
+  </si>
+  <si>
+    <t xml:space="preserve">欠 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> qiàn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> недостовать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">止 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> стопа, останавливаться</t>
+  </si>
+  <si>
+    <t xml:space="preserve">歹，歺 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dǎi </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> злой, плохой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">殳 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shū </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> бамбуковая пика</t>
+  </si>
+  <si>
+    <t xml:space="preserve">毋 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> нет, нельзя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">比 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> сравнивать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">毛 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> máo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> шерсть, волосы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">氏 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> род, клан</t>
+  </si>
+  <si>
+    <t xml:space="preserve">气 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> qì </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> воздух, газ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">水，氵，氺 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shuǐ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> вода</t>
+  </si>
+  <si>
+    <t xml:space="preserve">火，灬 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> huǒ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> огонь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">爪，爫 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zhăo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> когти</t>
+  </si>
+  <si>
+    <t xml:space="preserve">父 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fù </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> отец</t>
+  </si>
+  <si>
+    <t xml:space="preserve">爻 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yáo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> воздействие, влияние</t>
+  </si>
+  <si>
+    <t xml:space="preserve">爿，丬 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pán，qiáng </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> доска, кровать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">片 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> piàn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> карточка, щепка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">牙 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yá </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> зуб</t>
+  </si>
+  <si>
+    <t xml:space="preserve">牛 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> niú </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> корова</t>
+  </si>
+  <si>
+    <t xml:space="preserve">犬，犭 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> quăn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> собака</t>
+  </si>
+  <si>
+    <t xml:space="preserve">玄 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xuán </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> темный, тайный</t>
+  </si>
+  <si>
+    <t xml:space="preserve">玉 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yù </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> яшма</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瓜 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> guā </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> тыква, дыня</t>
+  </si>
+  <si>
+    <t xml:space="preserve">瓦 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wă </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> черепица</t>
+  </si>
+  <si>
+    <t xml:space="preserve">甘 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> сладкий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">生 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shēng </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> рождаться, сырой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">用，甩 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yòng </t>
+  </si>
+  <si>
+    <t xml:space="preserve">田 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tián </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> поле</t>
+  </si>
+  <si>
+    <t xml:space="preserve">疋 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pĭ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> нога, колено</t>
+  </si>
+  <si>
+    <t xml:space="preserve">疒 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chuáng </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> болезнь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">癶 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bō </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ноги врозь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">白 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bái </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> белый</t>
+  </si>
+  <si>
+    <t xml:space="preserve">皮 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pí </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> кожа, шкура</t>
+  </si>
+  <si>
+    <t xml:space="preserve">皿 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mĭn </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> блюдо, посуда</t>
+  </si>
+  <si>
+    <t xml:space="preserve">目 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> глаз</t>
+  </si>
+  <si>
+    <t xml:space="preserve">矛 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> копье</t>
+  </si>
+  <si>
+    <t xml:space="preserve">矢 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> shĭ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> стрела</t>
+  </si>
+  <si>
+    <t xml:space="preserve">石 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> камень</t>
+  </si>
+  <si>
+    <t xml:space="preserve">示，礻 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> алтарь, демонстрировать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">禸 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> róu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> след зверя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">禾 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hé </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> зерно, крупа</t>
+  </si>
+  <si>
+    <t xml:space="preserve">穴 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> xué </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> пещера</t>
+  </si>
+  <si>
+    <t xml:space="preserve">立 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> стоять</t>
+  </si>
+  <si>
+    <t xml:space="preserve">竹 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zhú </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> бамбук</t>
+  </si>
+  <si>
+    <t xml:space="preserve">米 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mĭ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> рис</t>
+  </si>
+  <si>
+    <t xml:space="preserve">纟，糹 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> нить, шелк</t>
+  </si>
+  <si>
+    <t xml:space="preserve">缶 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fŏu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> керамика, глиняная посуда</t>
+  </si>
+  <si>
+    <t xml:space="preserve">网，罒，罓 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wăng </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> сеть</t>
+  </si>
+  <si>
+    <t xml:space="preserve">羊 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yáng </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> баран</t>
+  </si>
+  <si>
+    <t xml:space="preserve">羽 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> yŭ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> перья, крылья</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> шагать вперед</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> медленно идти</t>
+  </si>
+  <si>
+    <t>использовать</t>
+  </si>
+  <si>
+    <t>восемь</t>
+  </si>
+  <si>
+    <t>один</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5509,6 +6584,22 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF303545"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -5527,10 +6618,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5546,8 +6638,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5561,6 +6656,76 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>53498</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>167930</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1" descr="Chineasy">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38647795-810B-43A0-A08E-488D69CC3F74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1">
+          <a:off x="5076348" y="15538450"/>
+          <a:ext cx="543402" cy="650530"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6738,7 +7903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D79124-9754-4A69-B150-B37F221C3809}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -7098,6 +8263,1395 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D23E59-844A-46A7-A5CE-4BBE9C40551F}">
+  <dimension ref="A1:H124"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1021</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1040</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1069</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C54" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C60" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C63" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C66" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C72" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C78" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C80" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C81" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C82" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C83" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C84" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C87" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C88" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C89" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B93" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C94" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C95" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B96" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C96" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C97" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C98" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C99" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C100" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C101" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C102" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C103" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C104" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C105" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C106" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C107" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C109" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C110" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C111" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C112" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C113" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C114" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B115" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C115" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C116" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C117" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B118" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C118" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B120" t="s">
+        <v>1057</v>
+      </c>
+      <c r="C120" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C121" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C122" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C123" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C124" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H8" r:id="rId1" xr:uid="{A902FD52-2B41-419D-AC21-B6947B9ECAFC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
middle of nem main menu
</commit_message>
<xml_diff>
--- a/Discover China 1 all vocabulary.xlsx
+++ b/Discover China 1 all vocabulary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Discover China\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF53653E-2360-40B7-89F4-D52ECD69C9DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0CA571-4540-49B4-B4C9-937EA53F2D3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="12" xr2:uid="{7EBEC6ED-38C4-453E-AFF8-D89EE891FB41}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <sheet name="unit 10" sheetId="10" r:id="rId10"/>
     <sheet name="unit 11" sheetId="11" r:id="rId11"/>
     <sheet name="unit 12" sheetId="12" r:id="rId12"/>
-    <sheet name="keys" sheetId="13" r:id="rId13"/>
+    <sheet name="radicals" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -6722,10 +6722,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8270,8 +8266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D23E59-844A-46A7-A5CE-4BBE9C40551F}">
   <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>